<commit_message>
change all save buttons for Extra details pop ups
</commit_message>
<xml_diff>
--- a/ExcelFiles/MedicalCertificate.xlsx
+++ b/ExcelFiles/MedicalCertificate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233D3F1-1FEB-4F26-8FBC-902AF37B429D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EDD9E0-99BF-4499-BA02-5C7F26996094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="2175" windowWidth="20265" windowHeight="9270" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -467,9 +467,6 @@
     <t>01-04-2025</t>
   </si>
   <si>
-    <t>30-07-2025</t>
-  </si>
-  <si>
     <t>release.manoj</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>Certificate</t>
+  </si>
+  <si>
+    <t>30-08-2025</t>
   </si>
 </sst>
 </file>
@@ -847,10 +847,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC4204-8ACE-4862-BC4B-50AE1C5531A5}">
   <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1185,10 +1185,10 @@
         <v>53</v>
       </c>
       <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>54</v>
@@ -1715,7 +1715,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1755,7 @@
         <v>139</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
         <v>136</v>
@@ -1882,7 +1882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AC1D6B-224B-4783-A36E-A1F1F63C8E2F}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1963,14 +1963,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2229,21 +2227,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E45471CC-9AFA-4147-A50A-01BCBC520F94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4E55A-6C67-4895-94E6-14C6B175BE34}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2268,9 +2265,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4E55A-6C67-4895-94E6-14C6B175BE34}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E45471CC-9AFA-4147-A50A-01BCBC520F94}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Medical certificate date change
</commit_message>
<xml_diff>
--- a/ExcelFiles/MedicalCertificate.xlsx
+++ b/ExcelFiles/MedicalCertificate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Riomed\Release_Server\Cellma4ClinicalAuto2\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EDD9E0-99BF-4499-BA02-5C7F26996094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768D77CC-AAAC-4DD8-ABCA-5C7938F74F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="2175" windowWidth="20265" windowHeight="9270" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
     <t>Certificate</t>
   </si>
   <si>
-    <t>30-08-2025</t>
+    <t>30-09-2025</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EA1B80-280E-4D26-AF18-E86A7C091F1D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1882,7 +1882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AC1D6B-224B-4783-A36E-A1F1F63C8E2F}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1972,6 +1972,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100957D2DE5FA4F58469907EC3226CC7D98" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="090753d51dfd09a1119d54c5de179dfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="563c2453-77f6-4899-a3ec-7eb6553b4f66" xmlns:ns3="c9416fa7-6169-4354-a691-3cfdebf72cd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c8570d9b0f0a7b9a0c34f8b658bbfee" ns2:_="" ns3:_="">
     <xsd:import namespace="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
@@ -2226,17 +2237,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="563c2453-77f6-4899-a3ec-7eb6553b4f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9416fa7-6169-4354-a691-3cfdebf72cd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FD4E55A-6C67-4895-94E6-14C6B175BE34}">
   <ds:schemaRefs>
@@ -2246,6 +2246,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E45471CC-9AFA-4147-A50A-01BCBC520F94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
+    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCB7D6A-E6F4-49F1-91EA-99C5773FBF86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2262,15 +2273,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E45471CC-9AFA-4147-A50A-01BCBC520F94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="563c2453-77f6-4899-a3ec-7eb6553b4f66"/>
-    <ds:schemaRef ds:uri="c9416fa7-6169-4354-a691-3cfdebf72cd6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>